<commit_message>
Added data/rows to the sample file.
</commit_message>
<xml_diff>
--- a/sample_excel_workbooks/team_data.xlsx
+++ b/sample_excel_workbooks/team_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>first_name</t>
   </si>
@@ -35,13 +35,43 @@
     <t>last_name</t>
   </si>
   <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
     <t>date_of_birth</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>weight</t>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Janice</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Kooler</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Sholer</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Jiang</t>
   </si>
 </sst>
 </file>
@@ -77,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,13 +401,98 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>11.5</v>
+      </c>
+      <c r="D2">
+        <v>180.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>29545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>10.4</v>
+      </c>
+      <c r="D3">
+        <v>160.30000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>33727</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>190.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>33669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>10.5</v>
+      </c>
+      <c r="D5">
+        <v>160.4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>32998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>11.5</v>
+      </c>
+      <c r="D6">
+        <v>140.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>34853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>